<commit_message>
Lots of little tweaks to sets
</commit_message>
<xml_diff>
--- a/SupersNew/matrices.xlsx
+++ b/SupersNew/matrices.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$75</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="176">
   <si>
     <t>Skirmisher</t>
   </si>
@@ -535,6 +535,21 @@
   </si>
   <si>
     <t>Insect Form</t>
+  </si>
+  <si>
+    <t>Ninja</t>
+  </si>
+  <si>
+    <t>Martial Artist</t>
+  </si>
+  <si>
+    <t>Immortal</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Devil</t>
   </si>
 </sst>
 </file>
@@ -900,11 +915,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H60" sqref="H60"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,43 +1006,43 @@
         <v>3</v>
       </c>
       <c r="H2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"M",""))</f>
+        <f t="shared" ref="H2:H33" si="0">LEN($P2)-LEN(SUBSTITUTE($P2,"M",""))</f>
         <v>1</v>
       </c>
       <c r="I2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"S",""))</f>
+        <f t="shared" ref="I2:I33" si="1">LEN($P2)-LEN(SUBSTITUTE($P2,"S",""))</f>
         <v>3</v>
       </c>
       <c r="J2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"R",""))</f>
+        <f t="shared" ref="J2:J33" si="2">LEN($P2)-LEN(SUBSTITUTE($P2,"R",""))</f>
         <v>3</v>
       </c>
       <c r="K2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"T",""))</f>
+        <f t="shared" ref="K2:K33" si="3">LEN($P2)-LEN(SUBSTITUTE($P2,"T",""))</f>
         <v>0</v>
       </c>
       <c r="L2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"W",""))</f>
+        <f t="shared" ref="L2:L33" si="4">LEN($P2)-LEN(SUBSTITUTE($P2,"W",""))</f>
         <v>2</v>
       </c>
       <c r="M2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"C",""))</f>
+        <f t="shared" ref="M2:M33" si="5">LEN($P2)-LEN(SUBSTITUTE($P2,"C",""))</f>
         <v>0</v>
       </c>
       <c r="N2" s="9">
-        <f>LEN($P2)-LEN(SUBSTITUTE($P2,"P",""))</f>
+        <f t="shared" ref="N2:N33" si="6">LEN($P2)-LEN(SUBSTITUTE($P2,"P",""))</f>
         <v>1</v>
       </c>
       <c r="O2" s="9">
-        <f>COUNTIF(H2:N2, "&gt;0" )</f>
+        <f t="shared" ref="O2:O33" si="7">COUNTIF(H2:N2, "&gt;0" )</f>
         <v>5</v>
       </c>
       <c r="P2" s="9" t="str">
-        <f>_xlfn.CONCAT(C2:G2)</f>
+        <f t="shared" ref="P2:P33" si="8">_xlfn.CONCAT(C2:G2)</f>
         <v>MS+3RS+2RS+3RW+2PW+0</v>
       </c>
       <c r="Q2" s="9">
-        <f>MAX(H2:N2)</f>
+        <f t="shared" ref="Q2:Q33" si="9">MAX(H2:N2)</f>
         <v>3</v>
       </c>
     </row>
@@ -1054,43 +1069,43 @@
         <v>90</v>
       </c>
       <c r="H3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N3" s="9">
-        <f>LEN($P3)-LEN(SUBSTITUTE($P3,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="O3" s="9">
-        <f>COUNTIF(H3:N3, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P3" s="9" t="str">
-        <f>_xlfn.CONCAT(C3:G3)</f>
+        <f t="shared" si="8"/>
         <v>MP+4MT+3PR+2RT+0CP+1</v>
       </c>
       <c r="Q3" s="9">
-        <f>MAX(H3:N3)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1117,43 +1132,43 @@
         <v>3</v>
       </c>
       <c r="H4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N4" s="9">
-        <f>LEN($P4)-LEN(SUBSTITUTE($P4,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O4" s="9">
-        <f>COUNTIF(H4:N4, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P4" s="9" t="str">
-        <f>_xlfn.CONCAT(C4:G4)</f>
+        <f t="shared" si="8"/>
         <v>MS+1RS+2RS+4RS+3PW+0</v>
       </c>
       <c r="Q4" s="9">
-        <f>MAX(H4:N4)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1180,43 +1195,43 @@
         <v>3</v>
       </c>
       <c r="H5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N5" s="9">
-        <f>LEN($P5)-LEN(SUBSTITUTE($P5,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O5" s="9">
-        <f>COUNTIF(H5:N5, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P5" s="9" t="str">
-        <f>_xlfn.CONCAT(C5:G5)</f>
+        <f t="shared" si="8"/>
         <v>MS+3RS+2RS+3RW+2PW+0</v>
       </c>
       <c r="Q5" s="9">
-        <f>MAX(H5:N5)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1243,43 +1258,43 @@
         <v>51</v>
       </c>
       <c r="H6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N6" s="9">
-        <f>LEN($P6)-LEN(SUBSTITUTE($P6,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O6" s="9">
-        <f>COUNTIF(H6:N6, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P6" s="9" t="str">
-        <f>_xlfn.CONCAT(C6:G6)</f>
+        <f t="shared" si="8"/>
         <v>MS+5RT+2MR+1RS+2PT+0</v>
       </c>
       <c r="Q6" s="9">
-        <f>MAX(H6:N6)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1306,43 +1321,43 @@
         <v>159</v>
       </c>
       <c r="H7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N7" s="9">
-        <f>LEN($P7)-LEN(SUBSTITUTE($P7,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O7" s="9">
-        <f>COUNTIF(H7:N7, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P7" s="9" t="str">
-        <f>_xlfn.CONCAT(C7:G7)</f>
+        <f t="shared" si="8"/>
         <v>MS+3MT+3RS+2RT+2TW+0</v>
       </c>
       <c r="Q7" s="9">
-        <f>MAX(H7:N7)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1369,43 +1384,43 @@
         <v>85</v>
       </c>
       <c r="H8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N8" s="9">
-        <f>LEN($P8)-LEN(SUBSTITUTE($P8,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O8" s="9">
-        <f>COUNTIF(H8:N8, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P8" s="9" t="str">
-        <f>_xlfn.CONCAT(C8:G8)</f>
+        <f t="shared" si="8"/>
         <v>MW+1RS+2RW+2SW+3CW+2</v>
       </c>
       <c r="Q8" s="9">
-        <f>MAX(H8:N8)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1432,43 +1447,43 @@
         <v>34</v>
       </c>
       <c r="H9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N9" s="9">
-        <f>LEN($P9)-LEN(SUBSTITUTE($P9,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O9" s="9">
-        <f>COUNTIF(H9:N9, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P9" s="9" t="str">
-        <f>_xlfn.CONCAT(C9:G9)</f>
+        <f t="shared" si="8"/>
         <v>MW+0RW+2RW+3RS+3PW+2</v>
       </c>
       <c r="Q9" s="9">
-        <f>MAX(H9:N9)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1495,43 +1510,43 @@
         <v>40</v>
       </c>
       <c r="H10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N10" s="9">
-        <f>LEN($P10)-LEN(SUBSTITUTE($P10,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="O10" s="9">
-        <f>COUNTIF(H10:N10, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P10" s="9" t="str">
-        <f>_xlfn.CONCAT(C10:G10)</f>
+        <f t="shared" si="8"/>
         <v>MR+2RS+0PR+2PR+3PW+3</v>
       </c>
       <c r="Q10" s="9">
-        <f>MAX(H10:N10)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1558,43 +1573,43 @@
         <v>45</v>
       </c>
       <c r="H11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N11">
-        <f>LEN($P11)-LEN(SUBSTITUTE($P11,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O11">
-        <f>COUNTIF(H11:N11, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P11" t="str">
-        <f>_xlfn.CONCAT(C11:G11)</f>
+        <f t="shared" si="8"/>
         <v>MS+4ST+3MS+2RS+0PT+1</v>
       </c>
       <c r="Q11" s="5">
-        <f>MAX(H11:N11)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1621,43 +1636,43 @@
         <v>34</v>
       </c>
       <c r="H12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N12" s="9">
-        <f>LEN($P12)-LEN(SUBSTITUTE($P12,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O12" s="9">
-        <f>COUNTIF(H12:N12, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P12" s="9" t="str">
-        <f>_xlfn.CONCAT(C12:G12)</f>
+        <f t="shared" si="8"/>
         <v>MW+2RW+2RS+2RW+2PW+2</v>
       </c>
       <c r="Q12" s="9">
-        <f>MAX(H12:N12)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1684,43 +1699,43 @@
         <v>45</v>
       </c>
       <c r="H13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>LEN($P13)-LEN(SUBSTITUTE($P13,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O13">
-        <f>COUNTIF(H13:N13, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P13" t="str">
-        <f>_xlfn.CONCAT(C13:G13)</f>
+        <f t="shared" si="8"/>
         <v>MS+4ST+3MS+2RS+0PT+1</v>
       </c>
       <c r="Q13" s="5">
-        <f>MAX(H13:N13)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1747,43 +1762,43 @@
         <v>51</v>
       </c>
       <c r="H14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f>LEN($P14)-LEN(SUBSTITUTE($P14,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O14">
-        <f>COUNTIF(H14:N14, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P14" t="str">
-        <f>_xlfn.CONCAT(C14:G14)</f>
+        <f t="shared" si="8"/>
         <v>MS+3MS+2MS+3RS+2PT+0</v>
       </c>
       <c r="Q14" s="5">
-        <f>MAX(H14:N14)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1810,43 +1825,43 @@
         <v>55</v>
       </c>
       <c r="H15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="N15" s="9">
-        <f>LEN($P15)-LEN(SUBSTITUTE($P15,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O15" s="9">
-        <f>COUNTIF(H15:N15, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P15" s="9" t="str">
-        <f>_xlfn.CONCAT(C15:G15)</f>
+        <f t="shared" si="8"/>
         <v>PS+0CR+1RS+1CW+3CP+5</v>
       </c>
       <c r="Q15" s="9">
-        <f>MAX(H15:N15)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1873,43 +1888,43 @@
         <v>62</v>
       </c>
       <c r="H16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N16" s="11">
-        <f>LEN($P16)-LEN(SUBSTITUTE($P16,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O16" s="11">
-        <f>COUNTIF(H16:N16, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P16" s="11" t="str">
-        <f>_xlfn.CONCAT(C16:G16)</f>
+        <f t="shared" si="8"/>
         <v>MS+1RS+1PS+4RW+3PW+1</v>
       </c>
       <c r="Q16" s="9">
-        <f>MAX(H16:N16)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -1936,43 +1951,43 @@
         <v>62</v>
       </c>
       <c r="H17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="M17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N17">
-        <f>LEN($P17)-LEN(SUBSTITUTE($P17,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O17">
-        <f>COUNTIF(H17:N17, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P17" t="str">
-        <f>_xlfn.CONCAT(C17:G17)</f>
+        <f t="shared" si="8"/>
         <v>MR+4RS+1RW+1RW+3PW+1</v>
       </c>
       <c r="Q17" s="5">
-        <f>MAX(H17:N17)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -1999,43 +2014,43 @@
         <v>3</v>
       </c>
       <c r="H18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N18" s="11">
-        <f>LEN($P18)-LEN(SUBSTITUTE($P18,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O18" s="11">
-        <f>COUNTIF(H18:N18, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P18" s="11" t="str">
-        <f>_xlfn.CONCAT(C18:G18)</f>
+        <f t="shared" si="8"/>
         <v>MS+1RS+1PS+4RW+3PW+0</v>
       </c>
       <c r="Q18" s="9">
-        <f>MAX(H18:N18)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -2062,43 +2077,43 @@
         <v>9</v>
       </c>
       <c r="H19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N19" s="4">
-        <f>LEN($P19)-LEN(SUBSTITUTE($P19,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O19" s="4">
-        <f>COUNTIF(H19:N19, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P19" s="4" t="str">
-        <f>_xlfn.CONCAT(C19:G19)</f>
+        <f t="shared" si="8"/>
         <v>MS+2RS+3RS+2RS+3CP+0</v>
       </c>
       <c r="Q19" s="5">
-        <f>MAX(H19:N19)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2125,43 +2140,43 @@
         <v>9</v>
       </c>
       <c r="H20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N20">
-        <f>LEN($P20)-LEN(SUBSTITUTE($P20,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O20">
-        <f>COUNTIF(H20:N20, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P20" t="str">
-        <f>_xlfn.CONCAT(C20:G20)</f>
+        <f t="shared" si="8"/>
         <v>RS+4MS+2RS+2RS+2CP+0</v>
       </c>
       <c r="Q20" s="5">
-        <f>MAX(H20:N20)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2188,43 +2203,43 @@
         <v>128</v>
       </c>
       <c r="H21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N21" s="9">
-        <f>LEN($P21)-LEN(SUBSTITUTE($P21,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O21" s="9">
-        <f>COUNTIF(H21:N21, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P21" s="9" t="str">
-        <f>_xlfn.CONCAT(C21:G21)</f>
+        <f t="shared" si="8"/>
         <v>RS+3MS+2RS+1RW+4CR+0</v>
       </c>
       <c r="Q21" s="9">
-        <f>MAX(H21:N21)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2251,43 +2266,43 @@
         <v>3</v>
       </c>
       <c r="H22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N22" s="11">
-        <f>LEN($P22)-LEN(SUBSTITUTE($P22,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O22" s="11">
-        <f>COUNTIF(H22:N22, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P22" s="11" t="str">
-        <f>_xlfn.CONCAT(C22:G22)</f>
+        <f t="shared" si="8"/>
         <v>MS+1RS+1PS+4RW+3PW+0</v>
       </c>
       <c r="Q22" s="9">
-        <f>MAX(H22:N22)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -2314,43 +2329,43 @@
         <v>90</v>
       </c>
       <c r="H23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N23" s="9">
-        <f>LEN($P23)-LEN(SUBSTITUTE($P23,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O23" s="9">
-        <f>COUNTIF(H23:N23, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P23" s="9" t="str">
-        <f>_xlfn.CONCAT(C23:G23)</f>
+        <f t="shared" si="8"/>
         <v>PW+2PS+3PR+2RW+2CP+1</v>
       </c>
       <c r="Q23" s="9">
-        <f>MAX(H23:N23)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2377,43 +2392,43 @@
         <v>74</v>
       </c>
       <c r="H24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N24" s="9">
-        <f>LEN($P24)-LEN(SUBSTITUTE($P24,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O24" s="9">
-        <f>COUNTIF(H24:N24, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P24" s="9" t="str">
-        <f>_xlfn.CONCAT(C24:G24)</f>
+        <f t="shared" si="8"/>
         <v>RS+0RS+2PS+2RW+3CP+3</v>
       </c>
       <c r="Q24" s="9">
-        <f>MAX(H24:N24)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -2440,43 +2455,43 @@
         <v>77</v>
       </c>
       <c r="H25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N25" s="9">
-        <f>LEN($P25)-LEN(SUBSTITUTE($P25,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="O25" s="9">
-        <f>COUNTIF(H25:N25, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P25" s="9" t="str">
-        <f>_xlfn.CONCAT(C25:G25)</f>
+        <f t="shared" si="8"/>
         <v>MP+0RS+2PS+4PR+2CP+2</v>
       </c>
       <c r="Q25" s="9">
-        <f>MAX(H25:N25)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2503,43 +2518,43 @@
         <v>3</v>
       </c>
       <c r="H26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="M26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N26" s="11">
-        <f>LEN($P26)-LEN(SUBSTITUTE($P26,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="O26" s="11">
-        <f>COUNTIF(H26:N26, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P26" s="11" t="str">
-        <f>_xlfn.CONCAT(C26:G26)</f>
+        <f t="shared" si="8"/>
         <v>MS+1RS+1PS+4RW+3PW+0</v>
       </c>
       <c r="Q26" s="9">
-        <f>MAX(H26:N26)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -2566,43 +2581,43 @@
         <v>45</v>
       </c>
       <c r="H27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N27" s="9">
-        <f>LEN($P27)-LEN(SUBSTITUTE($P27,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O27" s="9">
-        <f>COUNTIF(H27:N27, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P27" s="9" t="str">
-        <f>_xlfn.CONCAT(C27:G27)</f>
+        <f t="shared" si="8"/>
         <v>MS+2ST+2RS+3RS+2PT+1</v>
       </c>
       <c r="Q27" s="9">
-        <f>MAX(H27:N27)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2629,43 +2644,43 @@
         <v>133</v>
       </c>
       <c r="H28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N28" s="11">
-        <f>LEN($P28)-LEN(SUBSTITUTE($P28,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O28" s="11">
-        <f>COUNTIF(H28:N28, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P28" s="11" t="str">
-        <f>_xlfn.CONCAT(C28:G28)</f>
+        <f t="shared" si="8"/>
         <v>MS+0RW+1SW+2RW+3PW+4</v>
       </c>
       <c r="Q28" s="11">
-        <f>MAX(H28:N28)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2692,43 +2707,43 @@
         <v>85</v>
       </c>
       <c r="H29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="M29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="N29" s="11">
-        <f>LEN($P29)-LEN(SUBSTITUTE($P29,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O29" s="11">
-        <f>COUNTIF(H29:N29, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P29" s="11" t="str">
-        <f>_xlfn.CONCAT(C29:G29)</f>
+        <f t="shared" si="8"/>
         <v>MR+1SW+2SW+2CR+3CW+2</v>
       </c>
       <c r="Q29" s="11">
-        <f>MAX(H29:N29)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -2755,43 +2770,43 @@
         <v>85</v>
       </c>
       <c r="H30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="M30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N30" s="11">
-        <f>LEN($P30)-LEN(SUBSTITUTE($P30,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O30" s="11">
-        <f>COUNTIF(H30:N30, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P30" s="11" t="str">
-        <f>_xlfn.CONCAT(C30:G30)</f>
+        <f t="shared" si="8"/>
         <v>MW+1RS+2RW+2SW+3CW+2</v>
       </c>
       <c r="Q30" s="11">
-        <f>MAX(H30:N30)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2818,43 +2833,43 @@
         <v>128</v>
       </c>
       <c r="H31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N31" s="9">
-        <f>LEN($P31)-LEN(SUBSTITUTE($P31,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O31" s="9">
-        <f>COUNTIF(H31:N31, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P31" s="9" t="str">
-        <f>_xlfn.CONCAT(C31:G31)</f>
+        <f t="shared" si="8"/>
         <v>RS+3MS+2RS+1RW+4CR+0</v>
       </c>
       <c r="Q31" s="9">
-        <f>MAX(H31:N31)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -2881,43 +2896,43 @@
         <v>90</v>
       </c>
       <c r="H32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N32" s="9">
-        <f>LEN($P32)-LEN(SUBSTITUTE($P32,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="O32" s="9">
-        <f>COUNTIF(H32:N32, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P32" s="9" t="str">
-        <f>_xlfn.CONCAT(C32:G32)</f>
+        <f t="shared" si="8"/>
         <v>MP+4MT+3PR+2RT+0CP+1</v>
       </c>
       <c r="Q32" s="9">
-        <f>MAX(H32:N32)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
@@ -2944,43 +2959,43 @@
         <v>9</v>
       </c>
       <c r="H33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"M",""))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"S",""))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"R",""))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"T",""))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"W",""))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"C",""))</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N33">
-        <f>LEN($P33)-LEN(SUBSTITUTE($P33,"P",""))</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O33">
-        <f>COUNTIF(H33:N33, "&gt;0" )</f>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="P33" t="str">
-        <f>_xlfn.CONCAT(C33:G33)</f>
+        <f t="shared" si="8"/>
         <v>RS+4MS+2RS+2RS+2CP+0</v>
       </c>
       <c r="Q33" s="5">
-        <f>MAX(H33:N33)</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
     </row>
@@ -3007,43 +3022,43 @@
         <v>128</v>
       </c>
       <c r="H34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"M",""))</f>
+        <f t="shared" ref="H34:H74" si="10">LEN($P34)-LEN(SUBSTITUTE($P34,"M",""))</f>
         <v>1</v>
       </c>
       <c r="I34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"S",""))</f>
+        <f t="shared" ref="I34:I74" si="11">LEN($P34)-LEN(SUBSTITUTE($P34,"S",""))</f>
         <v>3</v>
       </c>
       <c r="J34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"R",""))</f>
+        <f t="shared" ref="J34:J74" si="12">LEN($P34)-LEN(SUBSTITUTE($P34,"R",""))</f>
         <v>4</v>
       </c>
       <c r="K34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"T",""))</f>
+        <f t="shared" ref="K34:K74" si="13">LEN($P34)-LEN(SUBSTITUTE($P34,"T",""))</f>
         <v>0</v>
       </c>
       <c r="L34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"W",""))</f>
+        <f t="shared" ref="L34:L74" si="14">LEN($P34)-LEN(SUBSTITUTE($P34,"W",""))</f>
         <v>1</v>
       </c>
       <c r="M34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"C",""))</f>
+        <f t="shared" ref="M34:M74" si="15">LEN($P34)-LEN(SUBSTITUTE($P34,"C",""))</f>
         <v>1</v>
       </c>
       <c r="N34" s="9">
-        <f>LEN($P34)-LEN(SUBSTITUTE($P34,"P",""))</f>
+        <f t="shared" ref="N34:N74" si="16">LEN($P34)-LEN(SUBSTITUTE($P34,"P",""))</f>
         <v>0</v>
       </c>
       <c r="O34" s="9">
-        <f>COUNTIF(H34:N34, "&gt;0" )</f>
+        <f t="shared" ref="O34:O65" si="17">COUNTIF(H34:N34, "&gt;0" )</f>
         <v>5</v>
       </c>
       <c r="P34" s="9" t="str">
-        <f>_xlfn.CONCAT(C34:G34)</f>
+        <f t="shared" ref="P34:P74" si="18">_xlfn.CONCAT(C34:G34)</f>
         <v>RS+3MS+2RS+1RW+4CR+0</v>
       </c>
       <c r="Q34" s="9">
-        <f>MAX(H34:N34)</f>
+        <f t="shared" ref="Q34:Q74" si="19">MAX(H34:N34)</f>
         <v>4</v>
       </c>
     </row>
@@ -3070,43 +3085,43 @@
         <v>85</v>
       </c>
       <c r="H35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="M35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N35" s="9">
-        <f>LEN($P35)-LEN(SUBSTITUTE($P35,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O35" s="9">
-        <f>COUNTIF(H35:N35, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P35" s="9" t="str">
-        <f>_xlfn.CONCAT(C35:G35)</f>
+        <f t="shared" si="18"/>
         <v>MW+1RW+3RS+2RW+2CW+2</v>
       </c>
       <c r="Q35" s="9">
-        <f>MAX(H35:N35)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -3133,43 +3148,43 @@
         <v>128</v>
       </c>
       <c r="H36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="L36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N36" s="9">
-        <f>LEN($P36)-LEN(SUBSTITUTE($P36,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="O36" s="9">
-        <f>COUNTIF(H36:N36, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P36" s="9" t="str">
-        <f>_xlfn.CONCAT(C36:G36)</f>
+        <f t="shared" si="18"/>
         <v>PS+3PT+3PS+2PR+2CR+0</v>
       </c>
       <c r="Q36" s="9">
-        <f>MAX(H36:N36)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -3196,43 +3211,43 @@
         <v>90</v>
       </c>
       <c r="H37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N37" s="9">
-        <f>LEN($P37)-LEN(SUBSTITUTE($P37,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O37" s="9">
-        <f>COUNTIF(H37:N37, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P37" s="9" t="str">
-        <f>_xlfn.CONCAT(C37:G37)</f>
+        <f t="shared" si="18"/>
         <v>MS+0MR+2PS+4RS+3CP+1</v>
       </c>
       <c r="Q37" s="9">
-        <f>MAX(H37:N37)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3259,43 +3274,43 @@
         <v>133</v>
       </c>
       <c r="H38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="M38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f>LEN($P38)-LEN(SUBSTITUTE($P38,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O38">
-        <f>COUNTIF(H38:N38, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P38" t="str">
-        <f>_xlfn.CONCAT(C38:G38)</f>
+        <f t="shared" si="18"/>
         <v>MS+0RW+1SW+2RW+3PW+4</v>
       </c>
       <c r="Q38" s="5">
-        <f>MAX(H38:N38)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -3322,43 +3337,43 @@
         <v>128</v>
       </c>
       <c r="H39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N39" s="9">
-        <f>LEN($P39)-LEN(SUBSTITUTE($P39,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O39" s="9">
-        <f>COUNTIF(H39:N39, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P39" s="9" t="str">
-        <f>_xlfn.CONCAT(C39:G39)</f>
+        <f t="shared" si="18"/>
         <v>MS+2MS+2PR+4RS+2CR+0</v>
       </c>
       <c r="Q39" s="9">
-        <f>MAX(H39:N39)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3385,43 +3400,43 @@
         <v>85</v>
       </c>
       <c r="H40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="M40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="N40">
-        <f>LEN($P40)-LEN(SUBSTITUTE($P40,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O40">
-        <f>COUNTIF(H40:N40, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P40" t="str">
-        <f>_xlfn.CONCAT(C40:G40)</f>
+        <f t="shared" si="18"/>
         <v>CP+2SW+2PW+2RW+2CW+2</v>
       </c>
       <c r="Q40" s="5">
-        <f>MAX(H40:N40)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -3448,43 +3463,43 @@
         <v>55</v>
       </c>
       <c r="H41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="N41" s="9">
-        <f>LEN($P41)-LEN(SUBSTITUTE($P41,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O41" s="9">
-        <f>COUNTIF(H41:N41, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P41" s="9" t="str">
-        <f>_xlfn.CONCAT(C41:G41)</f>
+        <f t="shared" si="18"/>
         <v>MP+0CS+1RS+1CR+3CP+5</v>
       </c>
       <c r="Q41" s="9">
-        <f>MAX(H41:N41)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3511,43 +3526,43 @@
         <v>45</v>
       </c>
       <c r="H42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="J42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="L42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N42" s="4">
-        <f>LEN($P42)-LEN(SUBSTITUTE($P42,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O42" s="4">
-        <f>COUNTIF(H42:N42, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P42" s="4" t="str">
-        <f>_xlfn.CONCAT(C42:G42)</f>
+        <f t="shared" si="18"/>
         <v>MS+4ST+3MS+2RS+0PT+1</v>
       </c>
       <c r="Q42" s="5">
-        <f>MAX(H42:N42)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -3574,43 +3589,43 @@
         <v>116</v>
       </c>
       <c r="H43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="L43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N43" s="9">
-        <f>LEN($P43)-LEN(SUBSTITUTE($P43,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O43" s="9">
-        <f>COUNTIF(H43:N43, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P43" s="9" t="str">
-        <f>_xlfn.CONCAT(C43:G43)</f>
+        <f t="shared" si="18"/>
         <v>MS+2RT+3RS+2RS+1PT+2</v>
       </c>
       <c r="Q43" s="9">
-        <f>MAX(H43:N43)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3637,43 +3652,43 @@
         <v>9</v>
       </c>
       <c r="H44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N44">
-        <f>LEN($P44)-LEN(SUBSTITUTE($P44,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="O44">
-        <f>COUNTIF(H44:N44, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P44" t="str">
-        <f>_xlfn.CONCAT(C44:G44)</f>
+        <f t="shared" si="18"/>
         <v>MS+3MP+4PS+1RS+2CP+0</v>
       </c>
       <c r="Q44" s="5">
-        <f>MAX(H44:N44)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3700,43 +3715,43 @@
         <v>90</v>
       </c>
       <c r="H45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N45">
-        <f>LEN($P45)-LEN(SUBSTITUTE($P45,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="O45">
-        <f>COUNTIF(H45:N45, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P45" t="str">
-        <f>_xlfn.CONCAT(C45:G45)</f>
+        <f t="shared" si="18"/>
         <v>MS+0MS+1PS+5PR+3CP+1</v>
       </c>
       <c r="Q45" s="5">
-        <f>MAX(H45:N45)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3763,43 +3778,43 @@
         <v>151</v>
       </c>
       <c r="H46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N46" s="9">
-        <f>LEN($P46)-LEN(SUBSTITUTE($P46,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O46" s="9">
-        <f>COUNTIF(H46:N46, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P46" s="9" t="str">
-        <f>_xlfn.CONCAT(C46:G46)</f>
+        <f t="shared" si="18"/>
         <v>MS+3RS+3RW+1RS+2CW+1</v>
       </c>
       <c r="Q46" s="9">
-        <f>MAX(H46:N46)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3826,43 +3841,43 @@
         <v>9</v>
       </c>
       <c r="H47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N47">
-        <f>LEN($P47)-LEN(SUBSTITUTE($P47,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O47">
-        <f>COUNTIF(H47:N47, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P47" t="str">
-        <f>_xlfn.CONCAT(C47:G47)</f>
+        <f t="shared" si="18"/>
         <v>MR+3MS+2RS+2RS+3CP+0</v>
       </c>
       <c r="Q47" s="5">
-        <f>MAX(H47:N47)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3889,43 +3904,43 @@
         <v>85</v>
       </c>
       <c r="H48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N48" s="9">
-        <f>LEN($P48)-LEN(SUBSTITUTE($P48,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O48" s="9">
-        <f>COUNTIF(H48:N48, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P48" s="9" t="str">
-        <f>_xlfn.CONCAT(C48:G48)</f>
+        <f t="shared" si="18"/>
         <v>MS+2RS+2RW+2RS+2CW+2</v>
       </c>
       <c r="Q48" s="9">
-        <f>MAX(H48:N48)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -3952,43 +3967,43 @@
         <v>151</v>
       </c>
       <c r="H49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="M49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N49" s="9">
-        <f>LEN($P49)-LEN(SUBSTITUTE($P49,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O49" s="9">
-        <f>COUNTIF(H49:N49, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P49" s="9" t="str">
-        <f>_xlfn.CONCAT(C49:G49)</f>
+        <f t="shared" si="18"/>
         <v>MW+3SW+2RS+2RW+2CW+1</v>
       </c>
       <c r="Q49" s="9">
-        <f>MAX(H49:N49)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4015,43 +4030,43 @@
         <v>140</v>
       </c>
       <c r="H50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="M50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N50" s="9">
-        <f>LEN($P50)-LEN(SUBSTITUTE($P50,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O50" s="9">
-        <f>COUNTIF(H50:N50, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P50" s="9" t="str">
-        <f>_xlfn.CONCAT(C50:G50)</f>
+        <f t="shared" si="18"/>
         <v>MS+0SW+1RW+3RW+3CW+3</v>
       </c>
       <c r="Q50" s="9">
-        <f>MAX(H50:N50)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4078,43 +4093,43 @@
         <v>85</v>
       </c>
       <c r="H51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N51" s="9">
-        <f>LEN($P51)-LEN(SUBSTITUTE($P51,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O51" s="9">
-        <f>COUNTIF(H51:N51, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P51" s="9" t="str">
-        <f>_xlfn.CONCAT(C51:G51)</f>
+        <f t="shared" si="18"/>
         <v>MS+2RS+2RW+2RS+2CW+2</v>
       </c>
       <c r="Q51" s="9">
-        <f>MAX(H51:N51)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4141,43 +4156,43 @@
         <v>116</v>
       </c>
       <c r="H52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="L52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N52" s="9">
-        <f>LEN($P52)-LEN(SUBSTITUTE($P52,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O52" s="9">
-        <f>COUNTIF(H52:N52, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P52" s="9" t="str">
-        <f>_xlfn.CONCAT(C52:G52)</f>
+        <f t="shared" si="18"/>
         <v>MS+2RT+3RS+2RS+1PT+2</v>
       </c>
       <c r="Q52" s="9">
-        <f>MAX(H52:N52)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4204,43 +4219,43 @@
         <v>85</v>
       </c>
       <c r="H53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="M53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N53" s="9">
-        <f>LEN($P53)-LEN(SUBSTITUTE($P53,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O53" s="9">
-        <f>COUNTIF(H53:N53, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P53" s="9" t="str">
-        <f>_xlfn.CONCAT(C53:G53)</f>
+        <f t="shared" si="18"/>
         <v>MW+1RW+3RS+2RW+2CW+2</v>
       </c>
       <c r="Q53" s="9">
-        <f>MAX(H53:N53)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4267,43 +4282,43 @@
         <v>3</v>
       </c>
       <c r="H54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N54" s="9">
-        <f>LEN($P54)-LEN(SUBSTITUTE($P54,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O54" s="9">
-        <f>COUNTIF(H54:N54, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P54" s="9" t="str">
-        <f>_xlfn.CONCAT(C54:G54)</f>
+        <f t="shared" si="18"/>
         <v>MS+3RS+2RS+3RW+2PW+0</v>
       </c>
       <c r="Q54" s="9">
-        <f>MAX(H54:N54)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4330,43 +4345,43 @@
         <v>90</v>
       </c>
       <c r="H55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="L55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N55" s="9">
-        <f>LEN($P55)-LEN(SUBSTITUTE($P55,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="O55" s="9">
-        <f>COUNTIF(H55:N55, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P55" s="9" t="str">
-        <f>_xlfn.CONCAT(C55:G55)</f>
+        <f t="shared" si="18"/>
         <v>MP+4MT+3PR+2RT+0CP+1</v>
       </c>
       <c r="Q55" s="9">
-        <f>MAX(H55:N55)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4393,43 +4408,43 @@
         <v>9</v>
       </c>
       <c r="H56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N56" s="9">
-        <f>LEN($P56)-LEN(SUBSTITUTE($P56,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O56" s="9">
-        <f>COUNTIF(H56:N56, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P56" s="9" t="str">
-        <f>_xlfn.CONCAT(C56:G56)</f>
+        <f t="shared" si="18"/>
         <v>MR+3MS+1RS+1RS+5CP+0</v>
       </c>
       <c r="Q56" s="9">
-        <f>MAX(H56:N56)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4456,43 +4471,43 @@
         <v>116</v>
       </c>
       <c r="H57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="L57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N57" s="9">
-        <f>LEN($P57)-LEN(SUBSTITUTE($P57,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O57" s="9">
-        <f>COUNTIF(H57:N57, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P57" s="9" t="str">
-        <f>_xlfn.CONCAT(C57:G57)</f>
+        <f t="shared" si="18"/>
         <v>MS+2MT+4RS+0RT+2PT+2</v>
       </c>
       <c r="Q57" s="9">
-        <f>MAX(H57:N57)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4519,43 +4534,43 @@
         <v>90</v>
       </c>
       <c r="H58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="J58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="L58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N58" s="9">
-        <f>LEN($P58)-LEN(SUBSTITUTE($P58,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="O58" s="9">
-        <f>COUNTIF(H58:N58, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P58" s="9" t="str">
-        <f>_xlfn.CONCAT(C58:G58)</f>
+        <f t="shared" si="18"/>
         <v>MP+4MT+3PR+2RT+0CP+1</v>
       </c>
       <c r="Q58" s="9">
-        <f>MAX(H58:N58)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4582,43 +4597,43 @@
         <v>45</v>
       </c>
       <c r="H59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="J59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>2</v>
       </c>
       <c r="L59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N59">
-        <f>LEN($P59)-LEN(SUBSTITUTE($P59,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O59">
-        <f>COUNTIF(H59:N59, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P59" t="str">
-        <f>_xlfn.CONCAT(C59:G59)</f>
+        <f t="shared" si="18"/>
         <v>MS+4ST+3MS+2RS+0PT+1</v>
       </c>
       <c r="Q59" s="5">
-        <f>MAX(H59:N59)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4645,43 +4660,43 @@
         <v>90</v>
       </c>
       <c r="H60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N60" s="9">
-        <f>LEN($P60)-LEN(SUBSTITUTE($P60,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="O60" s="9">
-        <f>COUNTIF(H60:N60, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P60" s="9" t="str">
-        <f>_xlfn.CONCAT(C60:G60)</f>
+        <f t="shared" si="18"/>
         <v>PW+2PS+3PR+2RW+2CP+1</v>
       </c>
       <c r="Q60" s="9">
-        <f>MAX(H60:N60)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4708,43 +4723,43 @@
         <v>77</v>
       </c>
       <c r="H61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N61" s="9">
-        <f>LEN($P61)-LEN(SUBSTITUTE($P61,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
       <c r="O61" s="9">
-        <f>COUNTIF(H61:N61, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P61" s="9" t="str">
-        <f>_xlfn.CONCAT(C61:G61)</f>
+        <f t="shared" si="18"/>
         <v>MP+0RS+2PS+4PR+2CP+2</v>
       </c>
       <c r="Q61" s="9">
-        <f>MAX(H61:N61)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4771,43 +4786,43 @@
         <v>62</v>
       </c>
       <c r="H62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="M62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N62">
-        <f>LEN($P62)-LEN(SUBSTITUTE($P62,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O62">
-        <f>COUNTIF(H62:N62, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P62" t="str">
-        <f>_xlfn.CONCAT(C62:G62)</f>
+        <f t="shared" si="18"/>
         <v>MR+2RS+0RW+4RW+3PW+1</v>
       </c>
       <c r="Q62" s="5">
-        <f>MAX(H62:N62)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -4834,43 +4849,43 @@
         <v>90</v>
       </c>
       <c r="H63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N63" s="9">
-        <f>LEN($P63)-LEN(SUBSTITUTE($P63,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O63" s="9">
-        <f>COUNTIF(H63:N63, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P63" s="9" t="str">
-        <f>_xlfn.CONCAT(C63:G63)</f>
+        <f t="shared" si="18"/>
         <v>SW+3RS+2RW+1RS+2CP+1</v>
       </c>
       <c r="Q63" s="9">
-        <f>MAX(H63:N63)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4897,43 +4912,43 @@
         <v>90</v>
       </c>
       <c r="H64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="K64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N64" s="11">
-        <f>LEN($P64)-LEN(SUBSTITUTE($P64,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O64" s="11">
-        <f>COUNTIF(H64:N64, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P64" s="11" t="str">
-        <f>_xlfn.CONCAT(C64:G64)</f>
+        <f t="shared" si="18"/>
         <v>SW+3RS+2RW+1RS+2CP+1</v>
       </c>
       <c r="Q64" s="11">
-        <f>MAX(H64:N64)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -4960,43 +4975,43 @@
         <v>85</v>
       </c>
       <c r="H65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="M65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="N65" s="11">
-        <f>LEN($P65)-LEN(SUBSTITUTE($P65,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O65" s="11">
-        <f>COUNTIF(H65:N65, "&gt;0" )</f>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="P65" s="11" t="str">
-        <f>_xlfn.CONCAT(C65:G65)</f>
+        <f t="shared" si="18"/>
         <v>MR+1SW+2SW+2CR+3CW+2</v>
       </c>
       <c r="Q65" s="11">
-        <f>MAX(H65:N65)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -5023,43 +5038,43 @@
         <v>38</v>
       </c>
       <c r="H66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="K66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="M66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N66" s="9">
-        <f>LEN($P66)-LEN(SUBSTITUTE($P66,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O66" s="9">
-        <f>COUNTIF(H66:N66, "&gt;0" )</f>
+        <f t="shared" ref="O66:O74" si="20">COUNTIF(H66:N66, "&gt;0" )</f>
         <v>5</v>
       </c>
       <c r="P66" s="9" t="str">
-        <f>_xlfn.CONCAT(C66:G66)</f>
+        <f t="shared" si="18"/>
         <v>MW+0RW+2PR+3RS+3PR+2</v>
       </c>
       <c r="Q66" s="9">
-        <f>MAX(H66:N66)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -5086,43 +5101,43 @@
         <v>90</v>
       </c>
       <c r="H67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="J67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N67" s="9">
-        <f>LEN($P67)-LEN(SUBSTITUTE($P67,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="O67" s="9">
-        <f>COUNTIF(H67:N67, "&gt;0" )</f>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="P67" s="9" t="str">
-        <f>_xlfn.CONCAT(C67:G67)</f>
+        <f t="shared" si="18"/>
         <v>MS+0MR+2PS+4RS+3CP+1</v>
       </c>
       <c r="Q67" s="9">
-        <f>MAX(H67:N67)</f>
+        <f t="shared" si="19"/>
         <v>3</v>
       </c>
     </row>
@@ -5149,43 +5164,43 @@
         <v>9</v>
       </c>
       <c r="H68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="I68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="J68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="N68">
-        <f>LEN($P68)-LEN(SUBSTITUTE($P68,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O68">
-        <f>COUNTIF(H68:N68, "&gt;0" )</f>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="P68" t="str">
-        <f>_xlfn.CONCAT(C68:G68)</f>
+        <f t="shared" si="18"/>
         <v>MS+4MS+4RS+0RS+2CP+0</v>
       </c>
       <c r="Q68" s="5">
-        <f>MAX(H68:N68)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
@@ -5212,143 +5227,395 @@
         <v>77</v>
       </c>
       <c r="H69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"M",""))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="I69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"S",""))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="J69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"R",""))</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="K69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"T",""))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"W",""))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="M69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"C",""))</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="N69">
-        <f>LEN($P69)-LEN(SUBSTITUTE($P69,"P",""))</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="O69">
-        <f>COUNTIF(H69:N69, "&gt;0" )</f>
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
       <c r="P69" t="str">
-        <f>_xlfn.CONCAT(C69:G69)</f>
+        <f t="shared" si="18"/>
         <v>CM+3CS+3CR+0RS+2CP+2</v>
       </c>
       <c r="Q69" s="5">
-        <f>MAX(H69:N69)</f>
+        <f t="shared" si="19"/>
         <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>131</v>
+        <v>171</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G70" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O70">
+        <f t="shared" ref="O70:O73" si="21">COUNTIF(H70:N70, "&gt;0" )</f>
+        <v>5</v>
+      </c>
+      <c r="P70" t="str">
+        <f t="shared" ref="P70:P73" si="22">_xlfn.CONCAT(C70:G70)</f>
+        <v>MS+2RS+2RW+2RS+2CW+2</v>
+      </c>
+      <c r="Q70" s="5">
+        <f t="shared" ref="Q70:Q73" si="23">MAX(H70:N70)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="P71" t="str">
+        <f t="shared" si="22"/>
+        <v>MS+3RS+3RW+1RS+2CW+1</v>
+      </c>
+      <c r="Q71" s="5">
+        <f t="shared" si="23"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="16"/>
+        <v>4</v>
+      </c>
+      <c r="O72">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="P72" t="str">
+        <f t="shared" si="22"/>
+        <v>MS+3PS+3PW+1PS+0CP+3</v>
+      </c>
+      <c r="Q72" s="5">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="O73">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="P73" t="str">
+        <f t="shared" si="22"/>
+        <v>PR+2RS+0RW+2RS+3CW+3</v>
+      </c>
+      <c r="Q73" s="5">
+        <f t="shared" si="23"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"M",""))</f>
-        <v>2</v>
-      </c>
-      <c r="I70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"S",""))</f>
-        <v>3</v>
-      </c>
-      <c r="J70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"R",""))</f>
-        <v>2</v>
-      </c>
-      <c r="K70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"T",""))</f>
-        <v>2</v>
-      </c>
-      <c r="L70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"W",""))</f>
-        <v>0</v>
-      </c>
-      <c r="M70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"C",""))</f>
-        <v>0</v>
-      </c>
-      <c r="N70">
-        <f>LEN($P70)-LEN(SUBSTITUTE($P70,"P",""))</f>
-        <v>1</v>
-      </c>
-      <c r="O70">
-        <f>COUNTIF(H70:N70, "&gt;0" )</f>
-        <v>5</v>
-      </c>
-      <c r="P70" t="str">
-        <f>_xlfn.CONCAT(C70:G70)</f>
+      <c r="H74">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="O74">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="P74" t="str">
+        <f t="shared" si="18"/>
         <v>MS+3MT+3RS+2RS+2PT+0</v>
       </c>
-      <c r="Q70" s="5">
-        <f>MAX(H70:N70)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H71">
-        <f>SUM(H2:H70)</f>
-        <v>83</v>
-      </c>
-      <c r="I71">
-        <f>SUM(I2:I70)</f>
-        <v>167</v>
-      </c>
-      <c r="J71">
-        <f>SUM(J2:J70)</f>
-        <v>167</v>
-      </c>
-      <c r="K71">
-        <f>SUM(K2:K70)</f>
+      <c r="Q74" s="5">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <f t="shared" ref="H75:N75" si="24">SUM(H2:H74)</f>
+        <v>86</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="24"/>
+        <v>178</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="24"/>
+        <v>177</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="24"/>
         <v>34</v>
       </c>
-      <c r="L71">
-        <f>SUM(L2:L70)</f>
-        <v>94</v>
-      </c>
-      <c r="M71">
-        <f>SUM(M2:M70)</f>
-        <v>51</v>
-      </c>
-      <c r="N71">
-        <f>SUM(N2:N70)</f>
-        <v>94</v>
+      <c r="L75">
+        <f t="shared" si="24"/>
+        <v>101</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="24"/>
+        <v>55</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="24"/>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:Q71">
-    <sortCondition ref="A2:A71"/>
-    <sortCondition ref="B2:B71"/>
+  <sortState ref="A2:Q75">
+    <sortCondition ref="A2:A75"/>
+    <sortCondition ref="B2:B75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>